<commit_message>
added audio and camera but graphics (glsurfaceview) is causing ANRs
</commit_message>
<xml_diff>
--- a/docs/x.xlsx
+++ b/docs/x.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="215">
   <si>
     <t>Processor</t>
   </si>
@@ -85,6 +85,9 @@
     <t>Properties</t>
   </si>
   <si>
+    <t>Features</t>
+  </si>
+  <si>
     <t>Available Keys</t>
   </si>
   <si>
@@ -157,6 +160,12 @@
     <t>hardware</t>
   </si>
   <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>can crash device (LG Ally)</t>
+  </si>
+  <si>
     <t>save?</t>
   </si>
   <si>
@@ -308,9 +317,6 @@
   </si>
   <si>
     <t>brand</t>
-  </si>
-  <si>
-    <t>can crash device (LG Ally)</t>
   </si>
   <si>
     <t>retrieving camera info can look like it's going to take a pic</t>
@@ -932,7 +938,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:Z102"/>
+  <dimension ref="B1:AA102"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -940,13 +946,13 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.572549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="23" min="3" style="1" width="11.3647058823529"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.5254901960784"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.7411764705882"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="5.88627450980392"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="1" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="24" min="3" style="1" width="11.4078431372549"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="14.6862745098039"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="10.5686274509804"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="12.7921568627451"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="5.90980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="1" width="9.34509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="3" outlineLevel="0" r="1"/>
@@ -983,6 +989,7 @@
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="70.1" outlineLevel="0" r="3" s="2">
       <c r="C3" s="2" t="s">
@@ -1045,25 +1052,28 @@
       <c r="V3" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="W3" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30.55" outlineLevel="0" r="4" s="9">
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -1071,54 +1081,55 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="N4" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
-      <c r="U4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="V4" s="10"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="5" s="9">
+      <c r="U4" s="10"/>
+      <c r="V4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="W4" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="5" s="9">
       <c r="C5" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="9" t="s">
+      <c r="I5" s="11" t="s">
         <v>41</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>17</v>
@@ -1130,345 +1141,348 @@
         <v>19</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="V5" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="33.55" outlineLevel="0" r="6" s="9">
       <c r="D6" s="11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="9" t="s">
         <v>55</v>
       </c>
+      <c r="H6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="K6" s="9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="7" s="9">
       <c r="D7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O7" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>16</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="35.8" outlineLevel="0" r="8" s="9">
       <c r="D8" s="11" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="9" s="9">
       <c r="D9" s="11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="W9" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z9" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="X9" s="0"/>
+      <c r="AA9" s="9" t="s">
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="63.4" outlineLevel="0" r="10" s="9">
       <c r="D10" s="11" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="W10" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z10" s="9" t="s">
         <v>110</v>
+      </c>
+      <c r="X10" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA10" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="29.85" outlineLevel="0" r="11" s="9">
       <c r="D11" s="11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="49.25" outlineLevel="0" r="12" s="9">
       <c r="D12" s="11" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" s="0"/>
+        <v>124</v>
+      </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z12" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.4" outlineLevel="0" r="13" s="9">
       <c r="D13" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z13" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
+      </c>
+      <c r="AA13" s="9" t="s">
+        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="54.45" outlineLevel="0" r="14" s="9">
       <c r="D14" s="11" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="15" s="9">
       <c r="D15" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16" s="9">
       <c r="D16" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -1476,26 +1490,27 @@
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="17" s="9">
       <c r="D17" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18" s="9">
       <c r="D18" s="11" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="19">
       <c r="D19" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1504,7 +1519,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
       <c r="D20" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -1513,105 +1528,105 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="26">
       <c r="F26" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="28.35" outlineLevel="0" r="32"/>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="31.5" outlineLevel="0" r="33" s="2">
       <c r="C33" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="34">
       <c r="D34" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="35">
       <c r="D35" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="36">
       <c r="D36" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="37">
       <c r="D37" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="38">
       <c r="D38" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="39">
       <c r="D39" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="40">
       <c r="D40" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="41">
       <c r="D41" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="42">
       <c r="D42" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="21.75" outlineLevel="0" r="55" s="2">
       <c r="C55" s="13" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
@@ -1619,130 +1634,130 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="56" s="2">
       <c r="C56" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="57">
       <c r="C57" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D57" s="14" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="58">
       <c r="C58" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D58" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="59">
       <c r="C59" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="60">
       <c r="C60" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="61">
       <c r="C61" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="62">
       <c r="C62" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="63">
       <c r="C63" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="64">
       <c r="C64" s="15" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="65">
       <c r="D65" s="14" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="71" s="2">
@@ -1753,189 +1768,189 @@
         <v>15</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="72">
       <c r="D72" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="73">
       <c r="D73" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="74">
       <c r="D74" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="75">
       <c r="D75" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="76">
       <c r="D76" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="77">
       <c r="D77" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="78">
       <c r="D78" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="79">
       <c r="D79" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="80">
       <c r="D80" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="84">
       <c r="C84" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E84" s="16"/>
       <c r="F84" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="85">
       <c r="C85" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D85" s="16" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E85" s="16"/>
       <c r="F85" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="86">
       <c r="C86" s="16" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F86" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="87">
       <c r="C87" s="16" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E87" s="16"/>
       <c r="F87" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="88">
       <c r="C88" s="16" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E88" s="16"/>
       <c r="F88" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="89">
       <c r="C89" s="16" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E89" s="16"/>
       <c r="F89" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="90">
       <c r="C90" s="16" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D90" s="16" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E90" s="16"/>
       <c r="F90" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="91">
       <c r="C91" s="16" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D91" s="16" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E91" s="16"/>
       <c r="F91" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="92">
       <c r="C92" s="16" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E92" s="16"/>
       <c r="F92" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="93">
       <c r="C93" s="16" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E93" s="16"/>
       <c r="F93" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="99">
       <c r="E99" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="100">
       <c r="C100" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="101">
       <c r="C101" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="102">
       <c r="C102" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -1964,7 +1979,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1989,7 +2004,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added sensors, introduced interface for getting contents (dumping values)
</commit_message>
<xml_diff>
--- a/docs/x.xlsx
+++ b/docs/x.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="218">
   <si>
     <t>Processor</t>
   </si>
@@ -439,6 +439,9 @@
     <t>font scaling factor</t>
   </si>
   <si>
+    <t>links to battery activities</t>
+  </si>
+  <si>
     <t>-- Current Values--</t>
   </si>
   <si>
@@ -476,6 +479,9 @@
   </si>
   <si>
     <t>% discovered indicator</t>
+  </si>
+  <si>
+    <t>LINKS TO SYSTEM ACTIVITIES</t>
   </si>
   <si>
     <t>Software</t>
@@ -949,13 +955,13 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.572549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="9.34509803921569"/>
-    <col collapsed="false" hidden="false" max="25" min="3" style="1" width="11.4078431372549"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="14.6862745098039"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="10.5686274509804"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="12.7921568627451"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="5.90980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="1" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="9.38039215686275"/>
+    <col collapsed="false" hidden="false" max="25" min="3" style="1" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="14.7490196078431"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="12.843137254902"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="5.93725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="1" width="9.38039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="3" outlineLevel="0" r="1"/>
@@ -1092,7 +1098,6 @@
       </c>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
-      <c r="Q4" s="0"/>
       <c r="R4" s="10" t="s">
         <v>35</v>
       </c>
@@ -1130,7 +1135,7 @@
       <c r="J5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="11" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="9" t="s">
@@ -1148,7 +1153,6 @@
       <c r="P5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="0"/>
       <c r="R5" s="9" t="s">
         <v>46</v>
       </c>
@@ -1193,7 +1197,7 @@
       <c r="J6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="11" t="s">
         <v>60</v>
       </c>
       <c r="L6" s="9" t="s">
@@ -1211,7 +1215,6 @@
       <c r="P6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="0"/>
       <c r="R6" s="9" t="s">
         <v>66</v>
       </c>
@@ -1235,7 +1238,7 @@
       <c r="H7" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="11" t="s">
         <v>73</v>
       </c>
       <c r="L7" s="9" t="s">
@@ -1253,7 +1256,6 @@
       <c r="P7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="0"/>
       <c r="R7" s="9" t="s">
         <v>77</v>
       </c>
@@ -1277,7 +1279,7 @@
       <c r="H8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="11" t="s">
         <v>84</v>
       </c>
       <c r="L8" s="9" t="s">
@@ -1312,7 +1314,7 @@
       <c r="H9" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="11" t="s">
         <v>95</v>
       </c>
       <c r="L9" s="9" t="s">
@@ -1331,7 +1333,6 @@
       <c r="S9" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="Y9" s="0"/>
       <c r="AB9" s="9" t="s">
         <v>101</v>
       </c>
@@ -1352,7 +1353,7 @@
       <c r="H10" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="11" t="s">
         <v>107</v>
       </c>
       <c r="L10" s="9" t="s">
@@ -1394,7 +1395,7 @@
       <c r="H11" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="11" t="s">
         <v>119</v>
       </c>
       <c r="L11" s="9" t="s">
@@ -1422,7 +1423,7 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="11" t="s">
         <v>126</v>
       </c>
       <c r="L12" s="9" t="s">
@@ -1445,7 +1446,7 @@
       <c r="G13" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="11" t="s">
         <v>133</v>
       </c>
       <c r="L13" s="9" t="s">
@@ -1468,25 +1469,28 @@
       <c r="G14" s="11" t="s">
         <v>139</v>
       </c>
+      <c r="K14" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="L14" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="15" s="9">
       <c r="D15" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="R15" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16" s="9">
@@ -1494,7 +1498,7 @@
         <v>47</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -1507,23 +1511,23 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="17" s="9">
       <c r="D17" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18" s="9">
       <c r="D18" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="19">
       <c r="D19" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1532,7 +1536,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
       <c r="D20" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -1541,22 +1545,27 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="26">
       <c r="F26" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="27">
+      <c r="I27" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="28.35" outlineLevel="0" r="32"/>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="31.5" outlineLevel="0" r="33" s="2">
       <c r="C33" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>26</v>
@@ -1564,21 +1573,21 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="34">
       <c r="D34" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="35">
       <c r="D35" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="36">
@@ -1586,7 +1595,7 @@
         <v>47</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="37">
@@ -1594,7 +1603,7 @@
         <v>67</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="38">
@@ -1602,44 +1611,44 @@
         <v>78</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="39">
       <c r="D39" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="40">
       <c r="D40" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="41">
       <c r="D41" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="42">
       <c r="D42" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="21.75" outlineLevel="0" r="55" s="2">
       <c r="C55" s="13" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
@@ -1647,13 +1656,13 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="56" s="2">
       <c r="C56" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>26</v>
@@ -1661,30 +1670,30 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="57">
       <c r="C57" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D57" s="14" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="58">
       <c r="C58" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D58" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="59">
@@ -1695,10 +1704,10 @@
         <v>47</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="60">
@@ -1709,68 +1718,68 @@
         <v>67</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="61">
       <c r="C61" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="62">
       <c r="C62" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D62" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="63">
       <c r="C63" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="64">
       <c r="C64" s="15" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="65">
       <c r="D65" s="14" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="71" s="2">
@@ -1781,16 +1790,16 @@
         <v>15</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="72">
@@ -1798,7 +1807,7 @@
         <v>61</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="73">
@@ -1826,7 +1835,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="77">
       <c r="D77" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="78">
@@ -1841,7 +1850,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="80">
       <c r="D80" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="84">
@@ -1849,69 +1858,69 @@
         <v>30</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E84" s="16"/>
       <c r="F84" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="85">
       <c r="C85" s="16" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D85" s="16" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E85" s="16"/>
       <c r="F85" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="86">
       <c r="C86" s="16" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F86" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="87">
       <c r="C87" s="16" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E87" s="16"/>
       <c r="F87" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="88">
       <c r="C88" s="16" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E88" s="16"/>
       <c r="F88" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="89">
       <c r="C89" s="16" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E89" s="16"/>
       <c r="F89" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="90">
       <c r="C90" s="16" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D90" s="16" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E90" s="16"/>
       <c r="F90" s="16"/>
@@ -1921,14 +1930,14 @@
         <v>78</v>
       </c>
       <c r="D91" s="16" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E91" s="16"/>
       <c r="F91" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="92">
       <c r="C92" s="16" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D92" s="16" t="s">
         <v>46</v>
@@ -1938,32 +1947,32 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="93">
       <c r="C93" s="16" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E93" s="16"/>
       <c r="F93" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="99">
       <c r="E99" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="100">
       <c r="C100" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="101">
       <c r="C101" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="102">
       <c r="C102" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1992,7 +2001,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.74901960784314"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2017,7 +2026,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.71372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.74901960784314"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added system group of elements. chachacha
</commit_message>
<xml_diff>
--- a/docs/x.xlsx
+++ b/docs/x.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="219">
   <si>
     <t>Processor</t>
   </si>
@@ -85,6 +85,9 @@
     <t>USB (Later)</t>
   </si>
   <si>
+    <t>uptime</t>
+  </si>
+  <si>
     <t>Platform</t>
   </si>
   <si>
@@ -97,13 +100,13 @@
     <t>Available Keys</t>
   </si>
   <si>
-    <t>Logcat</t>
+    <t>Logcat (deprecated)</t>
   </si>
   <si>
     <t>Identifiers</t>
   </si>
   <si>
-    <t>CONFIGURATION</t>
+    <t>CONFIGURATION (deprecated)</t>
   </si>
   <si>
     <t>icon</t>
@@ -163,319 +166,316 @@
     <t>android ver</t>
   </si>
   <si>
+    <t>--All--</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>can crash device (LG Ally)</t>
+  </si>
+  <si>
+    <t>save?</t>
+  </si>
+  <si>
+    <t>imsi</t>
+  </si>
+  <si>
+    <t>(has mcc and mnc)</t>
+  </si>
+  <si>
+    <t>features</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>dimensions in/cm</t>
+  </si>
+  <si>
+    <t>- renderer (opengl)</t>
+  </si>
+  <si>
+    <t>- Shitloads of values</t>
+  </si>
+  <si>
+    <t>codecs</t>
+  </si>
+  <si>
+    <t>- usages</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>- operator + numeric</t>
+  </si>
+  <si>
+    <t>- ip</t>
+  </si>
+  <si>
+    <t>- MAC</t>
+  </si>
+  <si>
+    <t>incremental ver</t>
+  </si>
+  <si>
+    <t>bogoMIPS</t>
+  </si>
+  <si>
+    <t>/proc/meminfo</t>
+  </si>
+  <si>
+    <t>cache</t>
+  </si>
+  <si>
+    <t>Density &amp; dpi</t>
+  </si>
+  <si>
+    <t>- version</t>
+  </si>
+  <si>
+    <t>- history (available?)</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>map link</t>
+  </si>
+  <si>
+    <t>- cdma/gsm/both</t>
+  </si>
+  <si>
+    <t>build fingerprint</t>
+  </si>
+  <si>
+    <t>ABI</t>
+  </si>
+  <si>
+    <t>Threshholds</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>dpi x &amp; y</t>
+  </si>
+  <si>
+    <t>- vendor</t>
+  </si>
+  <si>
+    <t>state (charge/dis)</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>- type (evdo)</t>
+  </si>
+  <si>
+    <t>- gateway</t>
+  </si>
+  <si>
+    <t>kernel</t>
+  </si>
+  <si>
+    <t>ABI2</t>
+  </si>
+  <si>
+    <t>- foreground</t>
+  </si>
+  <si>
+    <t>Sd-ext / extrenal_sd / sdcard-ext</t>
+  </si>
+  <si>
+    <t>max simultaneous touch</t>
+  </si>
+  <si>
+    <t>- max texture size</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>- baseband</t>
+  </si>
+  <si>
+    <t>- signal</t>
+  </si>
+  <si>
+    <t>bootloader</t>
+  </si>
+  <si>
+    <t>retrieving camera info can look like it's going to take a pic</t>
+  </si>
+  <si>
+    <t>Arch.</t>
+  </si>
+  <si>
+    <t>- visible</t>
+  </si>
+  <si>
+    <t>root?</t>
+  </si>
+  <si>
+    <t>refresh rate</t>
+  </si>
+  <si>
+    <t>- max texture units</t>
+  </si>
+  <si>
+    <t>technology (li-ion)</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>bssid</t>
+  </si>
+  <si>
+    <t>RIL ver</t>
+  </si>
+  <si>
+    <t>live data</t>
+  </si>
+  <si>
+    <t>retrieving opengl info can crash some devices</t>
+  </si>
+  <si>
+    <t>Impl.</t>
+  </si>
+  <si>
+    <t>- secondary server</t>
+  </si>
+  <si>
+    <t>sd mounted?</t>
+  </si>
+  <si>
+    <t>pixel/image format</t>
+  </si>
+  <si>
+    <t>- extensions</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>resolution</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>RIL barcode</t>
+  </si>
+  <si>
+    <t>Var.</t>
+  </si>
+  <si>
+    <t>- hidden</t>
+  </si>
+  <si>
+    <t>fps?</t>
+  </si>
+  <si>
+    <t>voltage</t>
+  </si>
+  <si>
+    <t>max range</t>
+  </si>
+  <si>
+    <t>opengl version</t>
+  </si>
+  <si>
+    <t>record live data</t>
+  </si>
+  <si>
+    <t>Part.</t>
+  </si>
+  <si>
+    <t>- content provider</t>
+  </si>
+  <si>
+    <t>logical density</t>
+  </si>
+  <si>
+    <t>-health</t>
+  </si>
+  <si>
+    <t>min delay</t>
+  </si>
+  <si>
+    <t>api level</t>
+  </si>
+  <si>
+    <t>save stuff!</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>- empty</t>
+  </si>
+  <si>
+    <t>font scaling factor</t>
+  </si>
+  <si>
+    <t>links to battery activities</t>
+  </si>
+  <si>
+    <t>-- Current Values--</t>
+  </si>
+  <si>
+    <t>device features</t>
+  </si>
+  <si>
+    <t>-- Current freq and % --</t>
+  </si>
+  <si>
+    <t>rotation/orientation</t>
+  </si>
+  <si>
+    <t>others not supported</t>
+  </si>
+  <si>
+    <t>build.display</t>
+  </si>
+  <si>
     <t>hardware</t>
   </si>
   <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>can crash device (LG Ally)</t>
-  </si>
-  <si>
-    <t>save?</t>
-  </si>
-  <si>
-    <t>imsi</t>
-  </si>
-  <si>
-    <t>(has mcc and mnc)</t>
-  </si>
-  <si>
-    <t>features</t>
-  </si>
-  <si>
-    <t>free</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>dimensions in/cm</t>
-  </si>
-  <si>
-    <t>- renderer (opengl)</t>
-  </si>
-  <si>
-    <t>- Shitloads of values</t>
-  </si>
-  <si>
-    <t>codecs</t>
-  </si>
-  <si>
-    <t>- usages</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>- operator + numeric</t>
-  </si>
-  <si>
-    <t>- ip</t>
-  </si>
-  <si>
-    <t>- MAC</t>
-  </si>
-  <si>
-    <t>incremental ver</t>
+    <t>---------</t>
+  </si>
+  <si>
+    <t>revision</t>
   </si>
   <si>
     <t>board</t>
   </si>
   <si>
-    <t>bogoMIPS</t>
-  </si>
-  <si>
-    <t>/proc/meminfo</t>
-  </si>
-  <si>
-    <t>cache</t>
-  </si>
-  <si>
-    <t>Density &amp; dpi</t>
-  </si>
-  <si>
-    <t>- version</t>
-  </si>
-  <si>
-    <t>- history (available?)</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>map link</t>
-  </si>
-  <si>
-    <t>- cdma/gsm/both</t>
-  </si>
-  <si>
-    <t>build fingerprint</t>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>mic</t>
   </si>
   <si>
     <t>device</t>
   </si>
   <si>
-    <t>ABI</t>
-  </si>
-  <si>
-    <t>Threshholds</t>
-  </si>
-  <si>
-    <t>sd</t>
-  </si>
-  <si>
-    <t>dpi x &amp; y</t>
-  </si>
-  <si>
-    <t>- vendor</t>
-  </si>
-  <si>
-    <t>state (charge/dis)</t>
-  </si>
-  <si>
-    <t>vendor</t>
-  </si>
-  <si>
-    <t>- type (evdo)</t>
-  </si>
-  <si>
-    <t>- gateway</t>
-  </si>
-  <si>
-    <t>kernel</t>
-  </si>
-  <si>
-    <t>--All--</t>
-  </si>
-  <si>
-    <t>ABI2</t>
-  </si>
-  <si>
-    <t>- foreground</t>
-  </si>
-  <si>
-    <t>Sd-ext / extrenal_sd / sdcard-ext</t>
-  </si>
-  <si>
-    <t>max simultaneous touch</t>
-  </si>
-  <si>
-    <t>- max texture size</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>- baseband</t>
-  </si>
-  <si>
-    <t>- signal</t>
-  </si>
-  <si>
-    <t>bootloader</t>
+    <t>freq range</t>
   </si>
   <si>
     <t>brand</t>
-  </si>
-  <si>
-    <t>retrieving camera info can look like it's going to take a pic</t>
-  </si>
-  <si>
-    <t>Arch.</t>
-  </si>
-  <si>
-    <t>- visible</t>
-  </si>
-  <si>
-    <t>root?</t>
-  </si>
-  <si>
-    <t>refresh rate</t>
-  </si>
-  <si>
-    <t>- max texture units</t>
-  </si>
-  <si>
-    <t>technology (li-ion)</t>
-  </si>
-  <si>
-    <t>power</t>
-  </si>
-  <si>
-    <t>bssid</t>
-  </si>
-  <si>
-    <t>RIL ver</t>
-  </si>
-  <si>
-    <t>uptime</t>
-  </si>
-  <si>
-    <t>live data</t>
-  </si>
-  <si>
-    <t>retrieving opengl info can crash some devices</t>
-  </si>
-  <si>
-    <t>Impl.</t>
-  </si>
-  <si>
-    <t>- secondary server</t>
-  </si>
-  <si>
-    <t>sd mounted?</t>
-  </si>
-  <si>
-    <t>pixel/image format</t>
-  </si>
-  <si>
-    <t>- extensions</t>
-  </si>
-  <si>
-    <t>temp</t>
-  </si>
-  <si>
-    <t>resolution</t>
-  </si>
-  <si>
-    <t>speed</t>
-  </si>
-  <si>
-    <t>RIL barcode</t>
-  </si>
-  <si>
-    <t>Var.</t>
-  </si>
-  <si>
-    <t>- hidden</t>
-  </si>
-  <si>
-    <t>fps?</t>
-  </si>
-  <si>
-    <t>voltage</t>
-  </si>
-  <si>
-    <t>max range</t>
-  </si>
-  <si>
-    <t>opengl version</t>
-  </si>
-  <si>
-    <t>record live data</t>
-  </si>
-  <si>
-    <t>Part.</t>
-  </si>
-  <si>
-    <t>- content provider</t>
-  </si>
-  <si>
-    <t>logical density</t>
-  </si>
-  <si>
-    <t>-health</t>
-  </si>
-  <si>
-    <t>min delay</t>
-  </si>
-  <si>
-    <t>api level</t>
-  </si>
-  <si>
-    <t>save stuff!</t>
-  </si>
-  <si>
-    <t>Revision</t>
-  </si>
-  <si>
-    <t>- empty</t>
-  </si>
-  <si>
-    <t>font scaling factor</t>
-  </si>
-  <si>
-    <t>links to battery activities</t>
-  </si>
-  <si>
-    <t>-- Current Values--</t>
-  </si>
-  <si>
-    <t>device features</t>
-  </si>
-  <si>
-    <t>-- Current freq and % --</t>
-  </si>
-  <si>
-    <t>rotation/orientation</t>
-  </si>
-  <si>
-    <t>others not supported</t>
-  </si>
-  <si>
-    <t>build.display</t>
-  </si>
-  <si>
-    <t>---------</t>
-  </si>
-  <si>
-    <t>revision</t>
-  </si>
-  <si>
-    <t>serial</t>
-  </si>
-  <si>
-    <t>mic</t>
-  </si>
-  <si>
-    <t>freq range</t>
   </si>
   <si>
     <t>freq stats</t>
@@ -714,7 +714,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -730,7 +730,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FF3366"/>
-        <bgColor rgb="00FF6600"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -755,6 +755,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="0033CC66"/>
         <bgColor rgb="00339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCC99"/>
+        <bgColor rgb="00C3D69B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF3366"/>
       </patternFill>
     </fill>
     <fill>
@@ -823,7 +835,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
@@ -849,28 +861,35 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="7" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="8" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="9" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="8" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="10" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="8" fontId="4" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="10" fontId="4" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="10" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="9" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="11" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="10" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="12" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="11" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="13" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -886,7 +905,7 @@
     <indexedColors>
       <rgbColor rgb="00000000"/>
       <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF3366"/>
+      <rgbColor rgb="00FF0000"/>
       <rgbColor rgb="0000FF00"/>
       <rgbColor rgb="000000FF"/>
       <rgbColor rgb="00FFFF00"/>
@@ -907,7 +926,7 @@
       <rgbColor rgb="00660066"/>
       <rgbColor rgb="00FF8080"/>
       <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00C3D69B"/>
       <rgbColor rgb="00000080"/>
       <rgbColor rgb="00FF00FF"/>
       <rgbColor rgb="00FFFF00"/>
@@ -923,13 +942,13 @@
       <rgbColor rgb="0083CAFF"/>
       <rgbColor rgb="00FF99CC"/>
       <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00C3D69B"/>
+      <rgbColor rgb="00FFCC99"/>
       <rgbColor rgb="003366FF"/>
       <rgbColor rgb="0033CC66"/>
       <rgbColor rgb="0099CC00"/>
       <rgbColor rgb="00FFD320"/>
       <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00FF3366"/>
       <rgbColor rgb="009966CC"/>
       <rgbColor rgb="00969696"/>
       <rgbColor rgb="00003366"/>
@@ -950,7 +969,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AC102"/>
+  <dimension ref="B1:AD102"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -959,12 +978,16 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.572549019607843"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="9.38039215686275"/>
-    <col collapsed="false" hidden="false" max="26" min="3" style="1" width="11.4588235294118"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="14.7490196078431"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="12.843137254902"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="5.93725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="9.38039215686275"/>
+    <col collapsed="false" hidden="false" max="23" min="3" style="1" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.1686274509804"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.8941176470588"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="14.7490196078431"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="12.843137254902"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="5.93725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="32" style="1" width="9.38039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="3" outlineLevel="0" r="1"/>
@@ -995,15 +1018,16 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="70.1" outlineLevel="0" r="3" s="2">
       <c r="C3" s="2" t="s">
@@ -1045,13 +1069,13 @@
       <c r="O3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="S3" s="2" t="s">
@@ -1069,477 +1093,498 @@
       <c r="W3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="X3" s="10" t="s">
         <v>27</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30.55" outlineLevel="0" r="4" s="9">
+      <c r="Z3" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30.55" outlineLevel="0" r="4" s="11">
       <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="N4" s="10" t="s">
+      <c r="G4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="S4" s="10" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="N4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10" t="s">
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="Y4" s="10"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="5" s="9">
-      <c r="C5" s="9" t="s">
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="Z4" s="12"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="5" s="11">
+      <c r="C5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="G5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="11" t="s">
+      <c r="I5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="J5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="11" t="s">
+      <c r="L5" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="M5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="S5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="U5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="V5" s="9" t="s">
+      <c r="V5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="W5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="X5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Y5" s="13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="33.55" outlineLevel="0" r="6" s="9">
-      <c r="D6" s="11" t="s">
+      <c r="Z5" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="12" t="s">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="33.55" outlineLevel="0" r="6" s="11">
+      <c r="D6" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="E6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="G6" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="H6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="I6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="J6" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="K6" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="L6" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="M6" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="N6" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="O6" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="Q6" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="S6" s="0"/>
+      <c r="T6" s="13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="7" s="9">
-      <c r="D7" s="11" t="s">
+      <c r="U6" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="7" s="11">
+      <c r="D7" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="S7" s="9" t="s">
+      <c r="O7" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="0"/>
+      <c r="T7" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="T7" s="9" t="s">
+      <c r="U7" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="35.8" outlineLevel="0" r="8" s="11">
+      <c r="D8" s="13" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="35.8" outlineLevel="0" r="8" s="9">
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="G8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H8" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="K8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="L8" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="N8" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="O8" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="S8" s="0"/>
+      <c r="T8" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="U8" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="9" s="11">
+      <c r="D9" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="E9" s="11" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="9" s="9">
-      <c r="D9" s="11" t="s">
+      <c r="F9" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="G9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="H9" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="K9" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="L9" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="N9" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="O9" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="O9" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-      <c r="S9" s="9" t="s">
+      <c r="S9" s="0"/>
+      <c r="T9" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="U9" s="0"/>
+      <c r="AD9" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="63.4" outlineLevel="0" r="10" s="11">
+      <c r="D10" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="T9" s="9" t="s">
+      <c r="E10" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="AC9" s="9" t="s">
+      <c r="F10" s="14" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="63.4" outlineLevel="0" r="10" s="9">
-      <c r="D10" s="11" t="s">
+      <c r="G10" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="H10" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="K10" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="L10" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="N10" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="O10" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="R10" s="2"/>
+      <c r="S10" s="0"/>
+      <c r="T10" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="AA10" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="N10" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="O10" s="11" t="s">
+      <c r="AD10" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="R10" s="2"/>
-      <c r="S10" s="9" t="s">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="29.85" outlineLevel="0" r="11" s="11">
+      <c r="D11" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="T10" s="9" t="s">
+      <c r="E11" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="Z10" s="9" t="s">
+      <c r="F11" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AC10" s="9" t="s">
+      <c r="G11" s="13" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="29.85" outlineLevel="0" r="11" s="9">
-      <c r="D11" s="11" t="s">
+      <c r="H11" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="K11" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="L11" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="N11" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="O11" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="S11" s="0"/>
+      <c r="T11" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="K11" s="11" t="s">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="49.25" outlineLevel="0" r="12" s="11">
+      <c r="D12" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="N11" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="O11" s="11" t="s">
+      <c r="G12" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="S11" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="49.25" outlineLevel="0" r="12" s="9">
-      <c r="D12" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="S12" s="0"/>
+      <c r="T12" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD12" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.4" outlineLevel="0" r="13" s="11">
+      <c r="D13" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="S12" s="9" t="s">
+      <c r="G13" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="AC12" s="9" t="s">
+      <c r="K13" s="13" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.4" outlineLevel="0" r="13" s="9">
-      <c r="D13" s="11" t="s">
+      <c r="L13" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="S13" s="0"/>
+      <c r="T13" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="AD13" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="K13" s="11" t="s">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="54.45" outlineLevel="0" r="14" s="11">
+      <c r="D14" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="S13" s="9" t="s">
+      <c r="G14" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="AC13" s="9" t="s">
+      <c r="K14" s="11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="54.45" outlineLevel="0" r="14" s="9">
-      <c r="D14" s="11" t="s">
+      <c r="L14" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="S14" s="0"/>
+      <c r="T14" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="G14" s="11" t="s">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="15" s="11">
+      <c r="D15" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="G15" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L15" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="S14" s="9" t="s">
+      <c r="S15" s="0"/>
+      <c r="T15" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="15" s="9">
-      <c r="D15" s="2" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16" s="11">
+      <c r="D16" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="L16" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="S15" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16" s="9">
-      <c r="D16" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>148</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
+      <c r="S16" s="0"/>
+      <c r="T16" s="13" t="s">
+        <v>144</v>
+      </c>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="17" s="9">
-      <c r="D17" s="11" t="s">
+      <c r="X16" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="17" s="11">
+      <c r="D17" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="S17" s="0"/>
+      <c r="T17" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18" s="11">
+      <c r="D18" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L18" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="L17" s="11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18" s="9">
-      <c r="D18" s="11" t="s">
+      <c r="S18" s="0"/>
+      <c r="T18" s="13" t="s">
         <v>150</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="19">
       <c r="D19" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="S19" s="0"/>
+      <c r="T19" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
       <c r="D20" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="26">
       <c r="F26" s="1" t="s">
@@ -1566,7 +1611,7 @@
         <v>159</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="34">
@@ -1590,7 +1635,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="36">
       <c r="D36" s="1" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>165</v>
@@ -1598,7 +1643,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="37">
       <c r="D37" s="1" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>166</v>
@@ -1606,7 +1651,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="38">
       <c r="D38" s="1" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>167</v>
@@ -1645,12 +1690,12 @@
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="21.75" outlineLevel="0" r="55" s="2">
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="56" s="2">
       <c r="C56" s="2" t="s">
@@ -1663,14 +1708,14 @@
         <v>178</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="57">
       <c r="C57" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D57" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="1" t="s">
@@ -1684,7 +1729,7 @@
       <c r="C58" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" s="17" t="s">
         <v>15</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -1699,7 +1744,7 @@
         <v>78</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>182</v>
@@ -1710,10 +1755,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="60">
       <c r="C60" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>183</v>
@@ -1726,10 +1771,10 @@
       <c r="C61" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="E61" s="18" t="s">
         <v>186</v>
       </c>
       <c r="F61" s="1" t="s">
@@ -1740,8 +1785,8 @@
       <c r="C62" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D62" s="14" t="s">
-        <v>31</v>
+      <c r="D62" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>188</v>
@@ -1762,10 +1807,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="64">
-      <c r="C64" s="15" t="s">
+      <c r="C64" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" s="17" t="s">
         <v>192</v>
       </c>
       <c r="F64" s="1" t="s">
@@ -1773,7 +1818,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="65">
-      <c r="D65" s="14" t="s">
+      <c r="D65" s="17" t="s">
         <v>194</v>
       </c>
       <c r="F65" s="1" t="s">
@@ -1791,7 +1836,7 @@
         <v>185</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>192</v>
@@ -1802,7 +1847,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="72">
       <c r="D72" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>197</v>
@@ -1813,22 +1858,22 @@
         <v>75</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="74">
       <c r="D74" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="75">
       <c r="D75" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="76">
       <c r="D76" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="77">
@@ -1838,12 +1883,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="78">
       <c r="D78" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="79">
       <c r="D79" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="80">
@@ -1852,106 +1897,106 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="84">
-      <c r="C84" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D84" s="16" t="s">
+      <c r="C84" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D84" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="85">
-      <c r="C85" s="16" t="s">
+      <c r="C85" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="D85" s="16" t="s">
+      <c r="D85" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="86">
-      <c r="C86" s="16" t="s">
+      <c r="C86" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="D86" s="16" t="s">
+      <c r="D86" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="E86" s="16" t="s">
+      <c r="E86" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="F86" s="16"/>
+      <c r="F86" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="87">
-      <c r="C87" s="16" t="s">
+      <c r="C87" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="D87" s="16" t="s">
+      <c r="D87" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="E87" s="16"/>
-      <c r="F87" s="16"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="88">
-      <c r="C88" s="16" t="s">
+      <c r="C88" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="D88" s="16" t="s">
+      <c r="D88" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="E88" s="16"/>
-      <c r="F88" s="16"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="89">
-      <c r="C89" s="16" t="s">
+      <c r="C89" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D89" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="E89" s="16"/>
-      <c r="F89" s="16"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="90">
-      <c r="C90" s="16" t="s">
+      <c r="C90" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="D90" s="16" t="s">
+      <c r="D90" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="E90" s="16"/>
-      <c r="F90" s="16"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="91">
-      <c r="C91" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D91" s="16" t="s">
+      <c r="C91" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D91" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="E91" s="16"/>
-      <c r="F91" s="16"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="92">
-      <c r="C92" s="16" t="s">
+      <c r="C92" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="D92" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E92" s="16"/>
-      <c r="F92" s="16"/>
+      <c r="D92" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="93">
-      <c r="C93" s="16" t="s">
+      <c r="C93" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="D93" s="16" t="s">
+      <c r="D93" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="E93" s="16"/>
-      <c r="F93" s="16"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="99">
       <c r="E99" s="1" t="s">

</xml_diff>

<commit_message>
not using loaders/db any more. trying to save/restore scrollview position but failing.
</commit_message>
<xml_diff>
--- a/docs/x.xlsx
+++ b/docs/x.xlsx
@@ -1192,7 +1192,7 @@
       <c r="V5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="W5" s="11" t="s">
+      <c r="W5" s="13" t="s">
         <v>51</v>
       </c>
       <c r="X5" s="11" t="s">
@@ -1565,7 +1565,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="19">
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="13" t="s">
         <v>151</v>
       </c>
       <c r="H19" s="11"/>
@@ -1578,7 +1578,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="13" t="s">
         <v>153</v>
       </c>
       <c r="H20" s="11"/>

</xml_diff>